<commit_message>
save progress exercises for stph workshop
</commit_message>
<xml_diff>
--- a/r_package/varia/input/noise_niph/example_road_noise_niph_test.xlsx
+++ b/r_package/varia/input/noise_niph/example_road_noise_niph_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luytax\switchdrive\BEST-COST\best-cost_WPs\r_package\testing\input\noise_niph\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luytax\switchdrive\BEST-COST\best-cost_WPs\r_package\varia\input\noise_niph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BAE96C-9C7D-4090-8DBF-A98195835AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843B697F-C17D-4940-9D82-62DF5FB446EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="12090" tabRatio="895" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="14490" tabRatio="895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Absolute_risk_HA" sheetId="21" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="36">
   <si>
     <t>&lt; 55</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>prop_pop_exp</t>
+  </si>
+  <si>
+    <t>prop_pop_exp of total population</t>
   </si>
 </sst>
 </file>
@@ -653,6 +656,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -662,10 +668,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -954,9 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1265,13 +1268,13 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.54296875" customWidth="1"/>
-    <col min="2" max="2" width="10.26953125" style="113" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" customWidth="1"/>
     <col min="3" max="3" width="18.453125" customWidth="1"/>
     <col min="4" max="4" width="19.54296875" customWidth="1"/>
     <col min="5" max="5" width="17.6328125" customWidth="1"/>
@@ -1314,7 +1317,9 @@
       <c r="I1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="3"/>
+      <c r="J1" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -1327,7 +1332,7 @@
       <c r="A2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="112"/>
+      <c r="B2" s="109"/>
       <c r="C2" s="46"/>
       <c r="D2" s="47"/>
       <c r="E2" s="29">
@@ -1337,7 +1342,10 @@
       <c r="F2" s="44"/>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
-      <c r="J2" s="6"/>
+      <c r="J2" s="113">
+        <f>E2/5213985</f>
+        <v>0.81871831238486492</v>
+      </c>
       <c r="K2" s="6"/>
       <c r="O2" s="7"/>
       <c r="P2" s="7"/>
@@ -1375,6 +1383,10 @@
       <c r="I3" s="1">
         <v>0.409966145</v>
       </c>
+      <c r="J3" s="113">
+        <f t="shared" ref="J3:J7" si="0">E3/5213985</f>
+        <v>7.4319354581956029E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
@@ -1390,7 +1402,7 @@
         <v>49500</v>
       </c>
       <c r="E4" s="30">
-        <f t="shared" ref="E4:E7" si="0">C4+D4</f>
+        <f t="shared" ref="E4:E7" si="1">C4+D4</f>
         <v>286000</v>
       </c>
       <c r="F4" s="51">
@@ -1402,11 +1414,15 @@
         <v>50788.594999999972</v>
       </c>
       <c r="H4" s="19">
-        <f t="shared" ref="H4:H6" si="1">G4*0.02</f>
+        <f t="shared" ref="H4:H6" si="2">G4*0.02</f>
         <v>1015.7718999999995</v>
       </c>
       <c r="I4" s="1">
         <v>0.30258146400000002</v>
+      </c>
+      <c r="J4" s="113">
+        <f t="shared" si="0"/>
+        <v>5.4852478478553353E-2</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
@@ -1423,7 +1439,7 @@
         <v>24500</v>
       </c>
       <c r="E5" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>191800</v>
       </c>
       <c r="F5" s="51">
@@ -1435,11 +1451,15 @@
         <v>46813.105500000063</v>
       </c>
       <c r="H5" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>936.26211000000126</v>
       </c>
       <c r="I5" s="1">
         <v>0.20292001700000001</v>
+      </c>
+      <c r="J5" s="113">
+        <f t="shared" si="0"/>
+        <v>3.6785683119533334E-2</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
@@ -1456,7 +1476,7 @@
         <v>2800</v>
       </c>
       <c r="E6" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>72200</v>
       </c>
       <c r="F6" s="51">
@@ -1468,11 +1488,15 @@
         <v>23657.232500000009</v>
       </c>
       <c r="H6" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>473.14465000000018</v>
       </c>
       <c r="I6" s="1">
         <v>7.6385949999999994E-2</v>
+      </c>
+      <c r="J6" s="113">
+        <f t="shared" si="0"/>
+        <v>1.384737393759284E-2</v>
       </c>
       <c r="M6" s="8"/>
     </row>
@@ -1490,7 +1514,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7700</v>
       </c>
       <c r="F7" s="51">
@@ -1507,6 +1531,10 @@
       </c>
       <c r="I7" s="1">
         <v>8.1464239999999993E-3</v>
+      </c>
+      <c r="J7" s="113">
+        <f t="shared" si="0"/>
+        <v>1.4767974974995133E-3</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
@@ -1578,6 +1606,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1585,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47139F8-AB47-402D-A7E6-875CE74C3AF2}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2462,9 +2491,9 @@
       <c r="N12" s="11"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="109"/>
-      <c r="B13" s="109"/>
-      <c r="C13" s="109"/>
+      <c r="A13" s="110"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="110"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="107"/>
@@ -2862,17 +2891,17 @@
       <c r="H12" s="71"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="110"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="110"/>
+      <c r="A13" s="111"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="111"/>
       <c r="F13" s="70"/>
       <c r="G13" s="70"/>
       <c r="H13" s="71"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="111"/>
-      <c r="B14" s="111"/>
-      <c r="C14" s="111"/>
+      <c r="A14" s="112"/>
+      <c r="B14" s="112"/>
+      <c r="C14" s="112"/>
       <c r="F14" s="72"/>
       <c r="G14" s="72"/>
       <c r="H14" s="71"/>
@@ -3298,17 +3327,17 @@
       <c r="H12" s="71"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="110"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="110"/>
+      <c r="A13" s="111"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="111"/>
       <c r="F13" s="70"/>
       <c r="G13" s="70"/>
       <c r="H13" s="71"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="111"/>
-      <c r="B14" s="111"/>
-      <c r="C14" s="111"/>
+      <c r="A14" s="112"/>
+      <c r="B14" s="112"/>
+      <c r="C14" s="112"/>
       <c r="F14" s="72"/>
       <c r="G14" s="72"/>
       <c r="H14" s="71"/>
@@ -3800,9 +3829,9 @@
       <c r="K12" s="71"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="110"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="110"/>
+      <c r="A13" s="111"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="111"/>
       <c r="F13" s="70"/>
       <c r="G13" s="70"/>
       <c r="H13" s="70"/>
@@ -3811,9 +3840,9 @@
       <c r="K13" s="71"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="111"/>
-      <c r="B14" s="111"/>
-      <c r="C14" s="111"/>
+      <c r="A14" s="112"/>
+      <c r="B14" s="112"/>
+      <c r="C14" s="112"/>
       <c r="F14" s="72"/>
       <c r="G14" s="72"/>
       <c r="H14" s="72"/>
@@ -3888,12 +3917,42 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FHI_TopicTaxHTField xmlns="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Støy</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8f2d7361-ae3f-42e5-b515-973ba07fa140</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Sykdomsbyrde</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">1cb2573e-d91b-47cf-a8ed-abd0332371f0</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Miljø og helse</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">87be7d37-248c-4b3c-9204-980558e4f787</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Miljøeksponering</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">d9196c48-ce51-47cd-b0d2-6ebc45d8709a</TermId>
+        </TermInfo>
+      </Terms>
+    </FHI_TopicTaxHTField>
+    <TaxCatchAll xmlns="e0a242cb-cec1-4671-aa99-615488d5530e">
+      <Value>15</Value>
+      <Value>10</Value>
+      <Value>2</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <TaxKeywordTaxHTField xmlns="e0a242cb-cec1-4671-aa99-615488d5530e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9d23e429-547e-4a13-8b71-070d02c5a1ec">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4135,48 +4194,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FHI_TopicTaxHTField xmlns="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Støy</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8f2d7361-ae3f-42e5-b515-973ba07fa140</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Sykdomsbyrde</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">1cb2573e-d91b-47cf-a8ed-abd0332371f0</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Miljø og helse</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">87be7d37-248c-4b3c-9204-980558e4f787</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Miljøeksponering</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">d9196c48-ce51-47cd-b0d2-6ebc45d8709a</TermId>
-        </TermInfo>
-      </Terms>
-    </FHI_TopicTaxHTField>
-    <TaxCatchAll xmlns="e0a242cb-cec1-4671-aa99-615488d5530e">
-      <Value>15</Value>
-      <Value>10</Value>
-      <Value>2</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <TaxKeywordTaxHTField xmlns="e0a242cb-cec1-4671-aa99-615488d5530e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9d23e429-547e-4a13-8b71-070d02c5a1ec">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A4E13C-9AD0-4A6A-9D51-20AD50148DE0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA136E82-55D6-4201-8C86-EA83CE955D86}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5"/>
+    <ds:schemaRef ds:uri="e0a242cb-cec1-4671-aa99-615488d5530e"/>
+    <ds:schemaRef ds:uri="9d23e429-547e-4a13-8b71-070d02c5a1ec"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4202,13 +4235,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA136E82-55D6-4201-8C86-EA83CE955D86}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A4E13C-9AD0-4A6A-9D51-20AD50148DE0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5"/>
-    <ds:schemaRef ds:uri="e0a242cb-cec1-4671-aa99-615488d5530e"/>
-    <ds:schemaRef ds:uri="9d23e429-547e-4a13-8b71-070d02c5a1ec"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
final version presentation for stph workshop
</commit_message>
<xml_diff>
--- a/r_package/varia/input/noise_niph/example_road_noise_niph_test.xlsx
+++ b/r_package/varia/input/noise_niph/example_road_noise_niph_test.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luytax\switchdrive\BEST-COST\best-cost_WPs\r_package\varia\input\noise_niph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843B697F-C17D-4940-9D82-62DF5FB446EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF44D699-3A4C-480F-84E1-C6E471733724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="14490" tabRatio="895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="14490" tabRatio="895" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Absolute_risk_HA" sheetId="21" r:id="rId1"/>
     <sheet name="Absolute_risk_HA_WS1_WP5" sheetId="24" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="25" r:id="rId3"/>
-    <sheet name="Absolute_risk_HSD" sheetId="18" r:id="rId4"/>
-    <sheet name="geo_id_1_rr_IHD_WHO_2003a" sheetId="22" r:id="rId5"/>
-    <sheet name="geo_id_2_rr_IHD_WHO_2003a" sheetId="19" r:id="rId6"/>
-    <sheet name="geo_id_3_rr_IHD_WHO_2003a (2)" sheetId="23" r:id="rId7"/>
-    <sheet name="Relative_risk_IHD_WHO_2003b" sheetId="20" r:id="rId8"/>
+    <sheet name="Sheet1" sheetId="26" r:id="rId4"/>
+    <sheet name="Absolute_risk_HSD" sheetId="18" r:id="rId5"/>
+    <sheet name="geo_id_1_rr_IHD_WHO_2003a" sheetId="22" r:id="rId6"/>
+    <sheet name="geo_id_2_rr_IHD_WHO_2003a" sheetId="19" r:id="rId7"/>
+    <sheet name="geo_id_3_rr_IHD_WHO_2003a (2)" sheetId="23" r:id="rId8"/>
+    <sheet name="Relative_risk_IHD_WHO_2003b" sheetId="20" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="43">
   <si>
     <t>&lt; 55</t>
   </si>
@@ -151,6 +152,27 @@
   </si>
   <si>
     <t>prop_pop_exp of total population</t>
+  </si>
+  <si>
+    <t>55 ≤ exp &lt; 60</t>
+  </si>
+  <si>
+    <t>exp &lt; 55</t>
+  </si>
+  <si>
+    <t>75 ≤ exp</t>
+  </si>
+  <si>
+    <t>70 ≤ exp &lt; 75</t>
+  </si>
+  <si>
+    <t>65 ≤ exp &lt; 70</t>
+  </si>
+  <si>
+    <t>60 ≤ exp &lt; 65</t>
+  </si>
+  <si>
+    <t>population_exposed</t>
   </si>
 </sst>
 </file>
@@ -476,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -659,6 +681,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -668,8 +693,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -959,7 +986,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1342,7 +1371,7 @@
       <c r="F2" s="44"/>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
-      <c r="J2" s="113">
+      <c r="J2" s="110">
         <f>E2/5213985</f>
         <v>0.81871831238486492</v>
       </c>
@@ -1383,7 +1412,7 @@
       <c r="I3" s="1">
         <v>0.409966145</v>
       </c>
-      <c r="J3" s="113">
+      <c r="J3" s="110">
         <f t="shared" ref="J3:J7" si="0">E3/5213985</f>
         <v>7.4319354581956029E-2</v>
       </c>
@@ -1420,7 +1449,7 @@
       <c r="I4" s="1">
         <v>0.30258146400000002</v>
       </c>
-      <c r="J4" s="113">
+      <c r="J4" s="110">
         <f t="shared" si="0"/>
         <v>5.4852478478553353E-2</v>
       </c>
@@ -1457,7 +1486,7 @@
       <c r="I5" s="1">
         <v>0.20292001700000001</v>
       </c>
-      <c r="J5" s="113">
+      <c r="J5" s="110">
         <f t="shared" si="0"/>
         <v>3.6785683119533334E-2</v>
       </c>
@@ -1494,7 +1523,7 @@
       <c r="I6" s="1">
         <v>7.6385949999999994E-2</v>
       </c>
-      <c r="J6" s="113">
+      <c r="J6" s="110">
         <f t="shared" si="0"/>
         <v>1.384737393759284E-2</v>
       </c>
@@ -1532,7 +1561,7 @@
       <c r="I7" s="1">
         <v>8.1464239999999993E-3</v>
       </c>
-      <c r="J7" s="113">
+      <c r="J7" s="110">
         <f t="shared" si="0"/>
         <v>1.4767974974995133E-3</v>
       </c>
@@ -1828,6 +1857,100 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A542A3-280B-40BF-B80F-43EAA2CF6BC9}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.36328125" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="3" max="3" width="21.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="18" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="116">
+        <v>4268785</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="114">
+        <v>57.5</v>
+      </c>
+      <c r="C3" s="8">
+        <v>387500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="114">
+        <v>62.5</v>
+      </c>
+      <c r="C4" s="8">
+        <v>286000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="114">
+        <v>67.5</v>
+      </c>
+      <c r="C5" s="8">
+        <v>191800</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="114">
+        <v>72.5</v>
+      </c>
+      <c r="C6" s="8">
+        <v>72200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="115">
+        <v>77.5</v>
+      </c>
+      <c r="C7" s="8">
+        <v>7700</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R9"/>
   <sheetViews>
@@ -2102,7 +2225,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N13"/>
   <sheetViews>
@@ -2491,9 +2614,9 @@
       <c r="N12" s="11"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="110"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="110"/>
+      <c r="A13" s="111"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="111"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
       <c r="F13" s="107"/>
@@ -2514,7 +2637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
@@ -2891,17 +3014,17 @@
       <c r="H12" s="71"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="111"/>
-      <c r="B13" s="111"/>
-      <c r="C13" s="111"/>
+      <c r="A13" s="112"/>
+      <c r="B13" s="112"/>
+      <c r="C13" s="112"/>
       <c r="F13" s="70"/>
       <c r="G13" s="70"/>
       <c r="H13" s="71"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="112"/>
-      <c r="B14" s="112"/>
-      <c r="C14" s="112"/>
+      <c r="A14" s="113"/>
+      <c r="B14" s="113"/>
+      <c r="C14" s="113"/>
       <c r="F14" s="72"/>
       <c r="G14" s="72"/>
       <c r="H14" s="71"/>
@@ -2950,7 +3073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
@@ -3327,17 +3450,17 @@
       <c r="H12" s="71"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="111"/>
-      <c r="B13" s="111"/>
-      <c r="C13" s="111"/>
+      <c r="A13" s="112"/>
+      <c r="B13" s="112"/>
+      <c r="C13" s="112"/>
       <c r="F13" s="70"/>
       <c r="G13" s="70"/>
       <c r="H13" s="71"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="112"/>
-      <c r="B14" s="112"/>
-      <c r="C14" s="112"/>
+      <c r="A14" s="113"/>
+      <c r="B14" s="113"/>
+      <c r="C14" s="113"/>
       <c r="F14" s="72"/>
       <c r="G14" s="72"/>
       <c r="H14" s="71"/>
@@ -3386,7 +3509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:R36"/>
   <sheetViews>
@@ -3829,9 +3952,9 @@
       <c r="K12" s="71"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="111"/>
-      <c r="B13" s="111"/>
-      <c r="C13" s="111"/>
+      <c r="A13" s="112"/>
+      <c r="B13" s="112"/>
+      <c r="C13" s="112"/>
       <c r="F13" s="70"/>
       <c r="G13" s="70"/>
       <c r="H13" s="70"/>
@@ -3840,9 +3963,9 @@
       <c r="K13" s="71"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="112"/>
-      <c r="B14" s="112"/>
-      <c r="C14" s="112"/>
+      <c r="A14" s="113"/>
+      <c r="B14" s="113"/>
+      <c r="C14" s="113"/>
       <c r="F14" s="72"/>
       <c r="G14" s="72"/>
       <c r="H14" s="72"/>
@@ -3956,6 +4079,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010000B17EB79AE2164A80F4AFE3B0051146" ma:contentTypeVersion="16" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="6bdb926755f4c89fc32634e0fb424225">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5" xmlns:ns3="e0a242cb-cec1-4671-aa99-615488d5530e" xmlns:ns4="9d23e429-547e-4a13-8b71-070d02c5a1ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0d894d6c78ef32a5fd57768bfb40a5e" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5"/>
@@ -4193,15 +4325,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA136E82-55D6-4201-8C86-EA83CE955D86}">
   <ds:schemaRefs>
@@ -4215,6 +4338,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A4E13C-9AD0-4A6A-9D51-20AD50148DE0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AF6BACD-FB0D-4A79-B41F-209A25C08460}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4232,12 +4363,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A4E13C-9AD0-4A6A-9D51-20AD50148DE0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
create new noise example data exdat_noise + adjust examples
</commit_message>
<xml_diff>
--- a/r_package/varia/input/noise_niph/example_road_noise_niph_test.xlsx
+++ b/r_package/varia/input/noise_niph/example_road_noise_niph_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luytax\switchdrive\BEST-COST\best-cost_WPs\r_package\varia\input\noise_niph\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF44D699-3A4C-480F-84E1-C6E471733724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5583E01C-6FA5-4BF2-B614-307B58E7A0C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="14490" tabRatio="895" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="14490" tabRatio="895" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Absolute_risk_HA" sheetId="21" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="49">
   <si>
     <t>&lt; 55</t>
   </si>
@@ -173,15 +173,34 @@
   </si>
   <si>
     <t>population_exposed</t>
+  </si>
+  <si>
+    <t>total rural</t>
+  </si>
+  <si>
+    <t>total urban</t>
+  </si>
+  <si>
+    <t>prop_pop_exp_urban</t>
+  </si>
+  <si>
+    <t>prop_pop_exp_total</t>
+  </si>
+  <si>
+    <t>urban &lt; 50</t>
+  </si>
+  <si>
+    <t>rural &lt; 50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.000000"/>
   </numFmts>
   <fonts count="32" x14ac:knownFonts="1">
     <font>
@@ -498,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -590,9 +609,6 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="17" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -684,6 +700,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -693,10 +714,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1044,10 +1069,10 @@
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58"/>
+      <c r="B2" s="57"/>
       <c r="C2" s="46"/>
       <c r="D2" s="47"/>
       <c r="E2" s="29">
@@ -1067,7 +1092,7 @@
       <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="59">
+      <c r="B3" s="58">
         <v>57.5</v>
       </c>
       <c r="C3" s="48">
@@ -1098,7 +1123,7 @@
       <c r="A4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="58">
         <v>62.5</v>
       </c>
       <c r="C4" s="48">
@@ -1129,7 +1154,7 @@
       <c r="A5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="59">
+      <c r="B5" s="58">
         <v>67.5</v>
       </c>
       <c r="C5" s="48">
@@ -1160,7 +1185,7 @@
       <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="59">
+      <c r="B6" s="58">
         <v>72.5</v>
       </c>
       <c r="C6" s="48">
@@ -1192,7 +1217,7 @@
       <c r="A7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="60">
+      <c r="B7" s="59">
         <v>77.5</v>
       </c>
       <c r="C7" s="48">
@@ -1252,7 +1277,7 @@
       <c r="N8" s="9"/>
     </row>
     <row r="9" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="56" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="22"/>
@@ -1296,7 +1321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88BAA2A8-1AEA-4C93-844A-28A4CEB1CB59}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -1358,10 +1383,10 @@
       <c r="Q1" s="4"/>
     </row>
     <row r="2" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="109"/>
+      <c r="B2" s="108"/>
       <c r="C2" s="46"/>
       <c r="D2" s="47"/>
       <c r="E2" s="29">
@@ -1371,7 +1396,7 @@
       <c r="F2" s="44"/>
       <c r="G2" s="17"/>
       <c r="H2" s="17"/>
-      <c r="J2" s="110">
+      <c r="J2" s="109">
         <f>E2/5213985</f>
         <v>0.81871831238486492</v>
       </c>
@@ -1412,7 +1437,7 @@
       <c r="I3" s="1">
         <v>0.409966145</v>
       </c>
-      <c r="J3" s="110">
+      <c r="J3" s="109">
         <f t="shared" ref="J3:J7" si="0">E3/5213985</f>
         <v>7.4319354581956029E-2</v>
       </c>
@@ -1449,7 +1474,7 @@
       <c r="I4" s="1">
         <v>0.30258146400000002</v>
       </c>
-      <c r="J4" s="110">
+      <c r="J4" s="109">
         <f t="shared" si="0"/>
         <v>5.4852478478553353E-2</v>
       </c>
@@ -1486,7 +1511,7 @@
       <c r="I5" s="1">
         <v>0.20292001700000001</v>
       </c>
-      <c r="J5" s="110">
+      <c r="J5" s="109">
         <f t="shared" si="0"/>
         <v>3.6785683119533334E-2</v>
       </c>
@@ -1523,7 +1548,7 @@
       <c r="I6" s="1">
         <v>7.6385949999999994E-2</v>
       </c>
-      <c r="J6" s="110">
+      <c r="J6" s="109">
         <f t="shared" si="0"/>
         <v>1.384737393759284E-2</v>
       </c>
@@ -1561,7 +1586,7 @@
       <c r="I7" s="1">
         <v>8.1464239999999993E-3</v>
       </c>
-      <c r="J7" s="110">
+      <c r="J7" s="109">
         <f t="shared" si="0"/>
         <v>1.4767974974995133E-3</v>
       </c>
@@ -1599,7 +1624,7 @@
       <c r="N8" s="9"/>
     </row>
     <row r="9" spans="1:17" ht="15.5" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="56" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="22"/>
@@ -1860,7 +1885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4A542A3-280B-40BF-B80F-43EAA2CF6BC9}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1883,10 +1908,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="116">
+      <c r="C2" s="112">
         <v>4268785</v>
       </c>
     </row>
@@ -1894,7 +1919,7 @@
       <c r="A3" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="114">
+      <c r="B3" s="110">
         <v>57.5</v>
       </c>
       <c r="C3" s="8">
@@ -1905,7 +1930,7 @@
       <c r="A4" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="114">
+      <c r="B4" s="110">
         <v>62.5</v>
       </c>
       <c r="C4" s="8">
@@ -1916,7 +1941,7 @@
       <c r="A5" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="114">
+      <c r="B5" s="110">
         <v>67.5</v>
       </c>
       <c r="C5" s="8">
@@ -1927,7 +1952,7 @@
       <c r="A6" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="114">
+      <c r="B6" s="110">
         <v>72.5</v>
       </c>
       <c r="C6" s="8">
@@ -1938,7 +1963,7 @@
       <c r="A7" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="115">
+      <c r="B7" s="111">
         <v>77.5</v>
       </c>
       <c r="C7" s="8">
@@ -1952,31 +1977,31 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD16"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="15.81640625" customWidth="1"/>
-    <col min="3" max="3" width="18.453125" customWidth="1"/>
-    <col min="4" max="4" width="19.54296875" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="15.7265625" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" customWidth="1"/>
-    <col min="8" max="8" width="13.54296875" customWidth="1"/>
-    <col min="11" max="11" width="13.1796875" customWidth="1"/>
-    <col min="12" max="12" width="23.54296875" customWidth="1"/>
-    <col min="13" max="13" width="21.54296875" customWidth="1"/>
-    <col min="14" max="14" width="21.453125" customWidth="1"/>
-    <col min="15" max="15" width="12.453125" customWidth="1"/>
-    <col min="17" max="17" width="10.453125" customWidth="1"/>
+    <col min="3" max="4" width="18.453125" customWidth="1"/>
+    <col min="5" max="6" width="19.54296875" customWidth="1"/>
+    <col min="7" max="8" width="15.453125" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" customWidth="1"/>
+    <col min="10" max="10" width="15.453125" customWidth="1"/>
+    <col min="11" max="11" width="13.54296875" customWidth="1"/>
+    <col min="14" max="14" width="13.1796875" customWidth="1"/>
+    <col min="15" max="15" width="23.54296875" customWidth="1"/>
+    <col min="16" max="16" width="21.54296875" customWidth="1"/>
+    <col min="17" max="17" width="21.453125" customWidth="1"/>
+    <col min="18" max="18" width="12.453125" customWidth="1"/>
+    <col min="20" max="20" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>15</v>
       </c>
@@ -1987,69 +2012,105 @@
         <v>14</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="H1" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="J1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="K1" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="12"/>
-    </row>
-    <row r="2" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="L1" s="12"/>
+    </row>
+    <row r="2" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="29">
-        <f>E9-E8</f>
+      <c r="B2" s="58"/>
+      <c r="C2" s="116">
+        <f>C16</f>
+        <v>3837204</v>
+      </c>
+      <c r="D2" s="117">
+        <f>C2/$C$9</f>
+        <v>0.86885257779858904</v>
+      </c>
+      <c r="E2" s="116">
+        <f>C17</f>
+        <v>708981</v>
+      </c>
+      <c r="F2" s="117">
+        <f>E2/$E$9</f>
+        <v>0.88891410402203663</v>
+      </c>
+      <c r="G2" s="29">
+        <f>G9-G8</f>
         <v>4546185</v>
       </c>
-      <c r="F2" s="43"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
-    </row>
-    <row r="3" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="H2" s="118">
+        <f>G2/$G$9</f>
+        <v>0.8719213806714059</v>
+      </c>
+      <c r="I2" s="43"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
+    </row>
+    <row r="3" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="59">
+      <c r="B3" s="58">
         <v>52.5</v>
       </c>
       <c r="C3" s="48">
         <v>264300</v>
       </c>
-      <c r="D3" s="48">
+      <c r="D3" s="117">
+        <f>C3/$C$9</f>
+        <v>5.9845068521810957E-2</v>
+      </c>
+      <c r="E3" s="48">
         <v>50700</v>
       </c>
-      <c r="E3" s="30">
-        <f>C3+D3</f>
+      <c r="F3" s="117">
+        <f t="shared" ref="F3:F7" si="0">E3/$E$9</f>
+        <v>6.356721135533569E-2</v>
+      </c>
+      <c r="G3" s="30">
+        <f>C3+E3</f>
         <v>315000</v>
       </c>
-      <c r="F3" s="51">
+      <c r="H3" s="118">
+        <f t="shared" ref="H3:H7" si="1">G3/$G$9</f>
+        <v>6.0414443079525544E-2</v>
+      </c>
+      <c r="I3" s="51">
         <f>19.4312-0.9336*B3+0.0126*B3^2</f>
         <v>5.1459500000000027</v>
       </c>
-      <c r="G3" s="30">
-        <f>E3*F3/100</f>
+      <c r="J3" s="30">
+        <f>G3*I3/100</f>
         <v>16209.742500000009</v>
       </c>
-      <c r="H3" s="30">
-        <f t="shared" ref="H3:H7" si="0">G3*0.07</f>
+      <c r="K3" s="30">
+        <f t="shared" ref="K3:K7" si="2">J3*0.07</f>
         <v>1134.6819750000009</v>
       </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
@@ -2057,128 +2118,179 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+    </row>
+    <row r="4" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="58">
         <v>57.5</v>
       </c>
       <c r="C4" s="48">
         <v>184700</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="117">
+        <f t="shared" ref="D4:D7" si="3">C4/$C$9</f>
+        <v>4.1821355111534182E-2</v>
+      </c>
+      <c r="E4" s="48">
         <v>32800</v>
       </c>
-      <c r="E4" s="30">
-        <f>C4+D4</f>
+      <c r="F4" s="117">
+        <f t="shared" si="0"/>
+        <v>4.1124349752564314E-2</v>
+      </c>
+      <c r="G4" s="30">
+        <f>C4+E4</f>
         <v>217500</v>
       </c>
-      <c r="F4" s="51">
+      <c r="H4" s="118">
+        <f t="shared" si="1"/>
+        <v>4.1714734507291448E-2</v>
+      </c>
+      <c r="I4" s="51">
         <f>19.4312-0.9336*B4+0.0126*B4^2</f>
         <v>7.4079499999999996</v>
       </c>
-      <c r="G4" s="30">
-        <f>E4*F4/100</f>
+      <c r="J4" s="30">
+        <f>G4*I4/100</f>
         <v>16112.29125</v>
       </c>
-      <c r="H4" s="30">
-        <f t="shared" si="0"/>
+      <c r="K4" s="30">
+        <f t="shared" si="2"/>
         <v>1127.8603875000001</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="59">
+      <c r="B5" s="58">
         <v>62.5</v>
       </c>
       <c r="C5" s="48">
         <v>107200</v>
       </c>
-      <c r="D5" s="48">
+      <c r="D5" s="117">
+        <f t="shared" si="3"/>
+        <v>2.4273141678161692E-2</v>
+      </c>
+      <c r="E5" s="48">
         <v>4300</v>
       </c>
-      <c r="E5" s="30">
-        <f>C5+D5</f>
+      <c r="F5" s="117">
+        <f t="shared" si="0"/>
+        <v>5.3913019492691028E-3</v>
+      </c>
+      <c r="G5" s="30">
+        <f>C5+E5</f>
         <v>111500</v>
       </c>
-      <c r="F5" s="51">
+      <c r="H5" s="118">
+        <f t="shared" si="1"/>
+        <v>2.1384794931324121E-2</v>
+      </c>
+      <c r="I5" s="51">
         <f>19.4312-0.9336*B5+0.0126*B5^2</f>
         <v>10.299949999999995</v>
       </c>
-      <c r="G5" s="30">
-        <f>E5*F5/100</f>
+      <c r="J5" s="30">
+        <f>G5*I5/100</f>
         <v>11484.444249999995</v>
       </c>
-      <c r="H5" s="30">
-        <f t="shared" si="0"/>
+      <c r="K5" s="30">
+        <f t="shared" si="2"/>
         <v>803.91109749999976</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="59">
+      <c r="B6" s="58">
         <v>67.5</v>
       </c>
       <c r="C6" s="48">
         <v>21600</v>
       </c>
-      <c r="D6" s="48">
+      <c r="D6" s="117">
+        <f t="shared" si="3"/>
+        <v>4.8908569053012357E-3</v>
+      </c>
+      <c r="E6" s="48">
         <v>800</v>
       </c>
-      <c r="E6" s="30">
-        <f>C6+D6</f>
+      <c r="F6" s="117">
+        <f t="shared" si="0"/>
+        <v>1.0030329207942517E-3</v>
+      </c>
+      <c r="G6" s="30">
+        <f>C6+E6</f>
         <v>22400</v>
       </c>
-      <c r="F6" s="51">
+      <c r="H6" s="118">
+        <f t="shared" si="1"/>
+        <v>4.2961381745440386E-3</v>
+      </c>
+      <c r="I6" s="51">
         <f>19.4312-0.9336*B6+0.0126*B6^2</f>
         <v>13.821950000000001</v>
       </c>
-      <c r="G6" s="30">
-        <f>E6*F6/100</f>
+      <c r="J6" s="30">
+        <f>G6*I6/100</f>
         <v>3096.1168000000007</v>
       </c>
-      <c r="H6" s="30">
-        <f t="shared" si="0"/>
+      <c r="K6" s="30">
+        <f t="shared" si="2"/>
         <v>216.72817600000008</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="60">
+      <c r="B7" s="59">
         <v>72.5</v>
       </c>
       <c r="C7" s="48">
         <v>1400</v>
       </c>
-      <c r="D7" s="48">
+      <c r="D7" s="117">
+        <f t="shared" si="3"/>
+        <v>3.169999846028579E-4</v>
+      </c>
+      <c r="E7" s="48">
         <v>0</v>
       </c>
-      <c r="E7" s="30">
-        <f>C7+D7</f>
+      <c r="F7" s="117">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="30">
+        <f>C7+E7</f>
         <v>1400</v>
       </c>
-      <c r="F7" s="51">
+      <c r="H7" s="118">
+        <f t="shared" si="1"/>
+        <v>2.6850863590900241E-4</v>
+      </c>
+      <c r="I7" s="51">
         <f>19.4312-0.9336*B7+0.0126*B7^2</f>
         <v>17.973950000000016</v>
       </c>
-      <c r="G7" s="30">
-        <f>E7*F7/100</f>
+      <c r="J7" s="30">
+        <f>G7*I7/100</f>
         <v>251.63530000000026</v>
       </c>
-      <c r="H7" s="30">
-        <f t="shared" si="0"/>
+      <c r="K7" s="30">
+        <f t="shared" si="2"/>
         <v>17.61447100000002</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
         <v>6</v>
       </c>
@@ -2187,37 +2299,95 @@
         <f>SUM(C3:C7)</f>
         <v>579200</v>
       </c>
-      <c r="D8" s="49">
-        <f>SUM(D3:D7)</f>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49">
+        <f>SUM(E3:E7)</f>
         <v>88600</v>
       </c>
-      <c r="E8" s="28">
-        <f>SUM(E3:E7)</f>
+      <c r="F8" s="49"/>
+      <c r="G8" s="28">
+        <f>SUM(G3:G7)</f>
         <v>667800</v>
       </c>
-      <c r="F8" s="52"/>
-      <c r="G8" s="53">
-        <f>SUM(G3:G7)</f>
+      <c r="H8" s="28"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="53">
+        <f>SUM(J3:J7)</f>
         <v>47154.230100000008</v>
       </c>
-      <c r="H8" s="54">
-        <f>G8*0.07</f>
+      <c r="K8" s="54">
+        <f>J8*0.07</f>
         <v>3300.796107000001</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="22"/>
-      <c r="C9" s="53"/>
+      <c r="C9" s="53">
+        <f>SUM(C2:C7)</f>
+        <v>4416404</v>
+      </c>
       <c r="D9" s="53"/>
-      <c r="E9" s="50">
+      <c r="E9" s="53">
+        <f>SUM(E2:E7)</f>
+        <v>797581</v>
+      </c>
+      <c r="F9" s="53"/>
+      <c r="G9" s="50">
         <v>5213985</v>
       </c>
-      <c r="F9" s="53"/>
-      <c r="G9" s="53"/>
-      <c r="H9" s="53"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <f>E8/C8</f>
+        <v>0.15296961325966851</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14">
+        <f>ROUND(G9*C13, 0)</f>
+        <v>797581</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15">
+        <f>ROUND(G9*(1-C13), 0)</f>
+        <v>4416404</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="8">
+        <f>4416404-C3-C4-C5-C6-C7</f>
+        <v>3837204</v>
+      </c>
+      <c r="E16">
+        <f>C14+C15</f>
+        <v>5213985</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="8">
+        <f>797581-E3-E4-E5-E6-E7</f>
+        <v>708981</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2239,302 +2409,302 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="75" t="s">
+      <c r="D1" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="75" t="s">
+      <c r="E1" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="77" t="s">
+      <c r="F1" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="77" t="s">
+      <c r="G1" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="75" t="s">
+      <c r="H1" s="74" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="77" t="s">
+      <c r="I1" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="77" t="s">
+      <c r="J1" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="77" t="s">
+      <c r="K1" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="78" t="s">
+      <c r="L1" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="78" t="s">
+      <c r="M1" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="78" t="s">
+      <c r="N1" s="77" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="80">
+      <c r="B2" s="79">
         <v>53</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="83">
+      <c r="C2" s="80"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="82">
         <f>E9-E8</f>
         <v>4268785</v>
       </c>
-      <c r="F2" s="84">
+      <c r="F2" s="83">
         <f>E2/E9</f>
         <v>0.81871831238486492</v>
       </c>
-      <c r="G2" s="85">
+      <c r="G2" s="84">
         <f>EXP((LN(1.08)/10)*(B2-53))</f>
         <v>1</v>
       </c>
-      <c r="H2" s="86">
+      <c r="H2" s="85">
         <f>F2*G2</f>
         <v>0.81871831238486492</v>
       </c>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="88">
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="87">
         <v>5269.46</v>
       </c>
-      <c r="M2" s="88">
+      <c r="M2" s="87">
         <v>80092.63</v>
       </c>
-      <c r="N2" s="88">
+      <c r="N2" s="87">
         <v>85362.08</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="87" t="s">
+      <c r="A3" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="89">
+      <c r="B3" s="88">
         <v>57.5</v>
       </c>
-      <c r="C3" s="90">
+      <c r="C3" s="89">
         <v>327900</v>
       </c>
-      <c r="D3" s="90">
+      <c r="D3" s="89">
         <v>59600</v>
       </c>
-      <c r="E3" s="88">
+      <c r="E3" s="87">
         <f>C3+D3</f>
         <v>387500</v>
       </c>
-      <c r="F3" s="84">
+      <c r="F3" s="83">
         <f>E3/E9</f>
         <v>7.4319354581956029E-2</v>
       </c>
-      <c r="G3" s="85">
+      <c r="G3" s="84">
         <f>EXP((LN(1.08)/10)*(B3-53))</f>
         <v>1.0352391558831511</v>
       </c>
-      <c r="H3" s="86">
+      <c r="H3" s="85">
         <f>F3*G3</f>
         <v>7.6938305903204759E-2</v>
       </c>
-      <c r="I3" s="87"/>
-      <c r="J3" s="87"/>
-      <c r="K3" s="87"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="11"/>
     </row>
     <row r="4" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="86" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="89">
+      <c r="B4" s="88">
         <v>62.5</v>
       </c>
-      <c r="C4" s="90">
+      <c r="C4" s="89">
         <v>236500</v>
       </c>
-      <c r="D4" s="90">
+      <c r="D4" s="89">
         <v>49500</v>
       </c>
-      <c r="E4" s="88">
+      <c r="E4" s="87">
         <f t="shared" ref="E4:E7" si="0">C4+D4</f>
         <v>286000</v>
       </c>
-      <c r="F4" s="84">
+      <c r="F4" s="83">
         <f>E4/E9</f>
         <v>5.4852478478553353E-2</v>
       </c>
-      <c r="G4" s="85">
+      <c r="G4" s="84">
         <f t="shared" ref="G4:G7" si="1">EXP((LN(1.08)/10)*(B4-53))</f>
         <v>1.0758520895846009</v>
       </c>
-      <c r="H4" s="86">
+      <c r="H4" s="85">
         <f t="shared" ref="H4:H7" si="2">F4*G4</f>
         <v>5.9013153590045976E-2</v>
       </c>
-      <c r="I4" s="87"/>
-      <c r="J4" s="87"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
       <c r="K4" s="11"/>
-      <c r="L4" s="91"/>
-      <c r="M4" s="91"/>
-      <c r="N4" s="91"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="90"/>
+      <c r="N4" s="90"/>
     </row>
     <row r="5" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="87" t="s">
+      <c r="A5" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="89">
+      <c r="B5" s="88">
         <v>67.5</v>
       </c>
-      <c r="C5" s="90">
+      <c r="C5" s="89">
         <v>167300</v>
       </c>
-      <c r="D5" s="90">
+      <c r="D5" s="89">
         <v>24500</v>
       </c>
-      <c r="E5" s="88">
+      <c r="E5" s="87">
         <f t="shared" si="0"/>
         <v>191800</v>
       </c>
-      <c r="F5" s="84">
+      <c r="F5" s="83">
         <f>E5/E9</f>
         <v>3.6785683119533334E-2</v>
       </c>
-      <c r="G5" s="85">
+      <c r="G5" s="84">
         <f t="shared" si="1"/>
         <v>1.1180582883538033</v>
       </c>
-      <c r="H5" s="86">
+      <c r="H5" s="85">
         <f t="shared" si="2"/>
         <v>4.1128537904550837E-2</v>
       </c>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
       <c r="K5" s="11"/>
-      <c r="L5" s="91"/>
-      <c r="M5" s="91"/>
-      <c r="N5" s="91"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
+      <c r="N5" s="90"/>
     </row>
     <row r="6" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="89">
+      <c r="B6" s="88">
         <v>72.5</v>
       </c>
-      <c r="C6" s="90">
+      <c r="C6" s="89">
         <v>69400</v>
       </c>
-      <c r="D6" s="90">
+      <c r="D6" s="89">
         <v>2800</v>
       </c>
-      <c r="E6" s="88">
+      <c r="E6" s="87">
         <f t="shared" si="0"/>
         <v>72200</v>
       </c>
-      <c r="F6" s="84">
+      <c r="F6" s="83">
         <f>E6/E9</f>
         <v>1.384737393759284E-2</v>
       </c>
-      <c r="G6" s="85">
+      <c r="G6" s="84">
         <f t="shared" si="1"/>
         <v>1.1619202567513689</v>
       </c>
-      <c r="H6" s="86">
+      <c r="H6" s="85">
         <f t="shared" si="2"/>
         <v>1.6089544280900085E-2</v>
       </c>
-      <c r="I6" s="87"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="87"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="91"/>
+      <c r="K6" s="86"/>
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
     </row>
     <row r="7" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="89">
+      <c r="B7" s="88">
         <v>77.5</v>
       </c>
-      <c r="C7" s="90">
+      <c r="C7" s="89">
         <v>7700</v>
       </c>
-      <c r="D7" s="90">
+      <c r="D7" s="89">
         <v>0</v>
       </c>
-      <c r="E7" s="88">
+      <c r="E7" s="87">
         <f t="shared" si="0"/>
         <v>7700</v>
       </c>
-      <c r="F7" s="84">
+      <c r="F7" s="83">
         <f>E7/E9</f>
         <v>1.4767974974995133E-3</v>
       </c>
-      <c r="G7" s="85">
+      <c r="G7" s="84">
         <f t="shared" si="1"/>
         <v>1.2075029514221076</v>
       </c>
-      <c r="H7" s="86">
+      <c r="H7" s="85">
         <f t="shared" si="2"/>
         <v>1.783237336883445E-3</v>
       </c>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
       <c r="N7" s="11"/>
     </row>
     <row r="8" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="93"/>
-      <c r="C8" s="94">
+      <c r="B8" s="92"/>
+      <c r="C8" s="93">
         <f>SUM(C3:C7)</f>
         <v>808800</v>
       </c>
-      <c r="D8" s="94">
+      <c r="D8" s="93">
         <f>SUM(D3:D7)</f>
         <v>136400</v>
       </c>
-      <c r="E8" s="95">
+      <c r="E8" s="94">
         <f>SUM(E3:E7)</f>
         <v>945200</v>
       </c>
-      <c r="F8" s="96">
+      <c r="F8" s="95">
         <f>E8/E9</f>
         <v>0.18128168761513505</v>
       </c>
-      <c r="G8" s="93"/>
-      <c r="H8" s="96">
+      <c r="G8" s="92"/>
+      <c r="H8" s="95">
         <f>SUM((F2*G2+F3*G3+F4*G4+F5*G5+F6*G6+F7*G7)-1)/(F2*G2+F3*G3+F4*G4+F5*G5+F6*G6+F7*G7)*100</f>
         <v>1.3486713310095881</v>
       </c>
-      <c r="I8" s="97">
+      <c r="I8" s="96">
         <f>L2*H8/100</f>
         <v>71.067696319017841</v>
       </c>
-      <c r="J8" s="97">
+      <c r="J8" s="96">
         <f>M2*H8/100</f>
         <v>1080.1863390615847</v>
       </c>
-      <c r="K8" s="97">
+      <c r="K8" s="96">
         <f>I8+J8</f>
         <v>1151.2540353806025</v>
       </c>
@@ -2543,35 +2713,35 @@
       <c r="N8" s="11"/>
     </row>
     <row r="9" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="98" t="s">
+      <c r="A9" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="98"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="100">
+      <c r="B9" s="97"/>
+      <c r="C9" s="98"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="99">
         <v>5213985</v>
       </c>
-      <c r="F9" s="101">
+      <c r="F9" s="100">
         <f>SUM(F2:F7)</f>
         <v>1</v>
       </c>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="98"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
       <c r="N9" s="11"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="102"/>
-      <c r="B10" s="102"/>
-      <c r="C10" s="103"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="103"/>
-      <c r="F10" s="104"/>
+      <c r="A10" s="101"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="103"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
       <c r="I10" s="11"/>
@@ -2582,14 +2752,14 @@
       <c r="N10" s="11"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="102"/>
-      <c r="B11" s="102"/>
-      <c r="C11" s="103"/>
-      <c r="D11" s="103"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="105"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="106"/>
+      <c r="A11" s="101"/>
+      <c r="B11" s="101"/>
+      <c r="C11" s="102"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="104"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
       <c r="I11" s="11"/>
       <c r="J11" s="11"/>
       <c r="K11" s="11"/>
@@ -2598,14 +2768,14 @@
       <c r="N11" s="11"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A12" s="102"/>
-      <c r="B12" s="102"/>
-      <c r="C12" s="103"/>
-      <c r="D12" s="103"/>
-      <c r="E12" s="103"/>
-      <c r="F12" s="107"/>
-      <c r="G12" s="107"/>
-      <c r="H12" s="108"/>
+      <c r="A12" s="101"/>
+      <c r="B12" s="101"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="106"/>
+      <c r="G12" s="106"/>
+      <c r="H12" s="107"/>
       <c r="I12" s="11"/>
       <c r="J12" s="11"/>
       <c r="K12" s="11"/>
@@ -2614,14 +2784,14 @@
       <c r="N12" s="11"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="111"/>
-      <c r="B13" s="111"/>
-      <c r="C13" s="111"/>
+      <c r="A13" s="113"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="113"/>
       <c r="D13" s="11"/>
       <c r="E13" s="11"/>
-      <c r="F13" s="107"/>
-      <c r="G13" s="107"/>
-      <c r="H13" s="108"/>
+      <c r="F13" s="106"/>
+      <c r="G13" s="106"/>
+      <c r="H13" s="107"/>
       <c r="I13" s="11"/>
       <c r="J13" s="11"/>
       <c r="K13" s="11"/>
@@ -2642,7 +2812,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2697,13 +2867,13 @@
       <c r="K1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="67" t="s">
+      <c r="L1" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="67" t="s">
+      <c r="M1" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="67" t="s">
+      <c r="N1" s="66" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2711,7 +2881,7 @@
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58">
+      <c r="B2" s="57">
         <f>53 + A12</f>
         <v>58</v>
       </c>
@@ -2725,7 +2895,7 @@
         <f>(E2/E9) + A16</f>
         <v>0.81871831238486492</v>
       </c>
-      <c r="G2" s="66">
+      <c r="G2" s="65">
         <f>EXP((LN(1.08)/10)*(B2-53))</f>
         <v>1.0392304845413265</v>
       </c>
@@ -2750,7 +2920,7 @@
       <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="59">
+      <c r="B3" s="58">
         <f xml:space="preserve"> 57.5 + A12</f>
         <v>62.5</v>
       </c>
@@ -2768,7 +2938,7 @@
         <f xml:space="preserve"> (E3/E9) + A16</f>
         <v>7.4319354581956029E-2</v>
       </c>
-      <c r="G3" s="66">
+      <c r="G3" s="65">
         <f>EXP((LN(1.08)/10)*(B3-53))</f>
         <v>1.0758520895846009</v>
       </c>
@@ -2784,7 +2954,7 @@
       <c r="A4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="58">
         <f xml:space="preserve"> 62.5 + A12</f>
         <v>67.5</v>
       </c>
@@ -2802,7 +2972,7 @@
         <f xml:space="preserve"> (E4/E9) + A16</f>
         <v>5.4852478478553353E-2</v>
       </c>
-      <c r="G4" s="66">
+      <c r="G4" s="65">
         <f t="shared" ref="G4:G7" si="1">EXP((LN(1.08)/10)*(B4-53))</f>
         <v>1.1180582883538033</v>
       </c>
@@ -2821,7 +2991,7 @@
       <c r="A5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="59">
+      <c r="B5" s="58">
         <f xml:space="preserve"> 67.5+ A12</f>
         <v>72.5</v>
       </c>
@@ -2839,7 +3009,7 @@
         <f xml:space="preserve"> (E5/E9) + A16</f>
         <v>3.6785683119533334E-2</v>
       </c>
-      <c r="G5" s="66">
+      <c r="G5" s="65">
         <f t="shared" si="1"/>
         <v>1.1619202567513689</v>
       </c>
@@ -2858,7 +3028,7 @@
       <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="59">
+      <c r="B6" s="58">
         <f xml:space="preserve"> 72.5+ A12</f>
         <v>77.5</v>
       </c>
@@ -2876,7 +3046,7 @@
         <f xml:space="preserve"> (E6/E9) + A16</f>
         <v>1.384737393759284E-2</v>
       </c>
-      <c r="G6" s="66">
+      <c r="G6" s="65">
         <f t="shared" si="1"/>
         <v>1.2075029514221076</v>
       </c>
@@ -2892,7 +3062,7 @@
       <c r="A7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="60">
+      <c r="B7" s="59">
         <f xml:space="preserve"> 77.5 + A12</f>
         <v>82.5</v>
       </c>
@@ -2910,7 +3080,7 @@
         <f xml:space="preserve"> (E7/E9) + A16</f>
         <v>1.4767974974995133E-3</v>
       </c>
-      <c r="G7" s="66">
+      <c r="G7" s="65">
         <f t="shared" si="1"/>
         <v>1.2548738772914785</v>
       </c>
@@ -2997,9 +3167,9 @@
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
@@ -3009,56 +3179,56 @@
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="71"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="70"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="112"/>
-      <c r="B13" s="112"/>
-      <c r="C13" s="112"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="71"/>
+      <c r="A13" s="114"/>
+      <c r="B13" s="114"/>
+      <c r="C13" s="114"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="70"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="113"/>
-      <c r="B14" s="113"/>
-      <c r="C14" s="113"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="71"/>
+      <c r="A14" s="115"/>
+      <c r="B14" s="115"/>
+      <c r="C14" s="115"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="70"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="62" t="s">
+      <c r="A15" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="56"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="55"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0</v>
       </c>
       <c r="B16" s="8"/>
-      <c r="C16" s="64"/>
+      <c r="C16" s="63"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="56"/>
-      <c r="C17" s="64"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="63"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B18" s="8"/>
-      <c r="C18" s="64"/>
+      <c r="C18" s="63"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B19" s="8"/>
-      <c r="C19" s="64"/>
+      <c r="C19" s="63"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="56"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="64"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
@@ -3133,13 +3303,13 @@
       <c r="K1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="67" t="s">
+      <c r="L1" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="67" t="s">
+      <c r="M1" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="67" t="s">
+      <c r="N1" s="66" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3147,7 +3317,7 @@
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58">
+      <c r="B2" s="57">
         <f>53 + A12</f>
         <v>63</v>
       </c>
@@ -3161,7 +3331,7 @@
         <f>(E2/E9) + A16</f>
         <v>0.81871831238486492</v>
       </c>
-      <c r="G2" s="66">
+      <c r="G2" s="65">
         <f>EXP((LN(1.08)/10)*(B2-53))</f>
         <v>1.08</v>
       </c>
@@ -3186,7 +3356,7 @@
       <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="59">
+      <c r="B3" s="58">
         <f xml:space="preserve"> 57.5 + A12</f>
         <v>67.5</v>
       </c>
@@ -3204,7 +3374,7 @@
         <f xml:space="preserve"> (E3/E9) + A16</f>
         <v>7.4319354581956029E-2</v>
       </c>
-      <c r="G3" s="66">
+      <c r="G3" s="65">
         <f>EXP((LN(1.08)/10)*(B3-53))</f>
         <v>1.1180582883538033</v>
       </c>
@@ -3220,7 +3390,7 @@
       <c r="A4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="58">
         <f xml:space="preserve"> 62.5 + A12</f>
         <v>72.5</v>
       </c>
@@ -3238,7 +3408,7 @@
         <f xml:space="preserve"> (E4/E9) + A16</f>
         <v>5.4852478478553353E-2</v>
       </c>
-      <c r="G4" s="66">
+      <c r="G4" s="65">
         <f t="shared" ref="G4:G7" si="1">EXP((LN(1.08)/10)*(B4-53))</f>
         <v>1.1619202567513689</v>
       </c>
@@ -3257,7 +3427,7 @@
       <c r="A5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="59">
+      <c r="B5" s="58">
         <f xml:space="preserve"> 67.5+ A12</f>
         <v>77.5</v>
       </c>
@@ -3275,7 +3445,7 @@
         <f xml:space="preserve"> (E5/E9) + A16</f>
         <v>3.6785683119533334E-2</v>
       </c>
-      <c r="G5" s="66">
+      <c r="G5" s="65">
         <f t="shared" si="1"/>
         <v>1.2075029514221076</v>
       </c>
@@ -3294,7 +3464,7 @@
       <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="59">
+      <c r="B6" s="58">
         <f xml:space="preserve"> 72.5+ A12</f>
         <v>82.5</v>
       </c>
@@ -3312,7 +3482,7 @@
         <f xml:space="preserve"> (E6/E9) + A16</f>
         <v>1.384737393759284E-2</v>
       </c>
-      <c r="G6" s="66">
+      <c r="G6" s="65">
         <f t="shared" si="1"/>
         <v>1.2548738772914785</v>
       </c>
@@ -3328,7 +3498,7 @@
       <c r="A7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="60">
+      <c r="B7" s="59">
         <f xml:space="preserve"> 77.5 + A12</f>
         <v>87.5</v>
       </c>
@@ -3346,7 +3516,7 @@
         <f xml:space="preserve"> (E7/E9) + A16</f>
         <v>1.4767974974995133E-3</v>
       </c>
-      <c r="G7" s="66">
+      <c r="G7" s="65">
         <f t="shared" si="1"/>
         <v>1.3041031875358762</v>
       </c>
@@ -3433,9 +3603,9 @@
       <c r="C11" s="13"/>
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="11">
@@ -3445,56 +3615,56 @@
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="71"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="70"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="112"/>
-      <c r="B13" s="112"/>
-      <c r="C13" s="112"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="71"/>
+      <c r="A13" s="114"/>
+      <c r="B13" s="114"/>
+      <c r="C13" s="114"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="70"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="113"/>
-      <c r="B14" s="113"/>
-      <c r="C14" s="113"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="71"/>
+      <c r="A14" s="115"/>
+      <c r="B14" s="115"/>
+      <c r="C14" s="115"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="70"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="62" t="s">
+      <c r="A15" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="63"/>
-      <c r="C15" s="56"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="55"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0</v>
       </c>
       <c r="B16" s="8"/>
-      <c r="C16" s="64"/>
+      <c r="C16" s="63"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="56"/>
-      <c r="C17" s="64"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="63"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B18" s="8"/>
-      <c r="C18" s="64"/>
+      <c r="C18" s="63"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B19" s="8"/>
-      <c r="C19" s="64"/>
+      <c r="C19" s="63"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="56"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="64"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
@@ -3578,13 +3748,13 @@
       <c r="N1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="67" t="s">
+      <c r="O1" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="67" t="s">
+      <c r="P1" s="66" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="67" t="s">
+      <c r="Q1" s="66" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3592,7 +3762,7 @@
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="58">
+      <c r="B2" s="57">
         <v>53</v>
       </c>
       <c r="C2" s="46"/>
@@ -3605,20 +3775,20 @@
         <f>E2/E9</f>
         <v>0.81871831238486492</v>
       </c>
-      <c r="G2" s="66">
+      <c r="G2" s="65">
         <f>EXP((LN(1.08)/10)*(B2-53))</f>
         <v>1</v>
       </c>
-      <c r="H2" s="66">
+      <c r="H2" s="65">
         <f t="shared" ref="H2:H7" si="0">G2-1</f>
         <v>0</v>
       </c>
-      <c r="I2" s="66">
+      <c r="I2" s="65">
         <f t="shared" ref="I2:I7" si="1">F2*H2</f>
         <v>0</v>
       </c>
-      <c r="J2" s="66"/>
-      <c r="K2" s="73">
+      <c r="J2" s="65"/>
+      <c r="K2" s="72">
         <f>F2*G2</f>
         <v>0.81871831238486492</v>
       </c>
@@ -3639,7 +3809,7 @@
       <c r="A3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="59">
+      <c r="B3" s="58">
         <v>57.5</v>
       </c>
       <c r="C3" s="48">
@@ -3656,20 +3826,20 @@
         <f>E3/E9</f>
         <v>7.4319354581956029E-2</v>
       </c>
-      <c r="G3" s="66">
+      <c r="G3" s="65">
         <f>EXP((LN(1.08)/10)*(B3-53))</f>
         <v>1.0352391558831511</v>
       </c>
-      <c r="H3" s="66">
+      <c r="H3" s="65">
         <f t="shared" si="0"/>
         <v>3.5239155883151074E-2</v>
       </c>
-      <c r="I3" s="66">
+      <c r="I3" s="65">
         <f t="shared" si="1"/>
         <v>2.6189513212487264E-3</v>
       </c>
-      <c r="J3" s="66"/>
-      <c r="K3" s="73">
+      <c r="J3" s="65"/>
+      <c r="K3" s="72">
         <f>F3*G3</f>
         <v>7.6938305903204759E-2</v>
       </c>
@@ -3681,7 +3851,7 @@
       <c r="A4" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="59">
+      <c r="B4" s="58">
         <v>62.5</v>
       </c>
       <c r="C4" s="48">
@@ -3698,20 +3868,20 @@
         <f>E4/E9</f>
         <v>5.4852478478553353E-2</v>
       </c>
-      <c r="G4" s="66">
+      <c r="G4" s="65">
         <f t="shared" ref="G4:G7" si="3">EXP((LN(1.08)/10)*(B4-53))</f>
         <v>1.0758520895846009</v>
       </c>
-      <c r="H4" s="66">
+      <c r="H4" s="65">
         <f t="shared" si="0"/>
         <v>7.5852089584600879E-2</v>
       </c>
-      <c r="I4" s="66">
+      <c r="I4" s="65">
         <f t="shared" si="1"/>
         <v>4.1606751114926207E-3</v>
       </c>
-      <c r="J4" s="66"/>
-      <c r="K4" s="73">
+      <c r="J4" s="65"/>
+      <c r="K4" s="72">
         <f t="shared" ref="K4:K7" si="4">F4*G4</f>
         <v>5.9013153590045976E-2</v>
       </c>
@@ -3726,7 +3896,7 @@
       <c r="A5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="59">
+      <c r="B5" s="58">
         <v>67.5</v>
       </c>
       <c r="C5" s="48">
@@ -3743,20 +3913,20 @@
         <f>E5/E9</f>
         <v>3.6785683119533334E-2</v>
       </c>
-      <c r="G5" s="66">
+      <c r="G5" s="65">
         <f t="shared" si="3"/>
         <v>1.1180582883538033</v>
       </c>
-      <c r="H5" s="66">
+      <c r="H5" s="65">
         <f t="shared" si="0"/>
         <v>0.11805828835380328</v>
       </c>
-      <c r="I5" s="66">
+      <c r="I5" s="65">
         <f t="shared" si="1"/>
         <v>4.3428547850174999E-3</v>
       </c>
-      <c r="J5" s="66"/>
-      <c r="K5" s="73">
+      <c r="J5" s="65"/>
+      <c r="K5" s="72">
         <f t="shared" si="4"/>
         <v>4.1128537904550837E-2</v>
       </c>
@@ -3771,7 +3941,7 @@
       <c r="A6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="59">
+      <c r="B6" s="58">
         <v>72.5</v>
       </c>
       <c r="C6" s="48">
@@ -3788,20 +3958,20 @@
         <f>E6/E9</f>
         <v>1.384737393759284E-2</v>
       </c>
-      <c r="G6" s="66">
+      <c r="G6" s="65">
         <f t="shared" si="3"/>
         <v>1.1619202567513689</v>
       </c>
-      <c r="H6" s="66">
+      <c r="H6" s="65">
         <f t="shared" si="0"/>
         <v>0.1619202567513689</v>
       </c>
-      <c r="I6" s="66">
+      <c r="I6" s="65">
         <f t="shared" si="1"/>
         <v>2.2421703433072467E-3</v>
       </c>
-      <c r="J6" s="66"/>
-      <c r="K6" s="73">
+      <c r="J6" s="65"/>
+      <c r="K6" s="72">
         <f t="shared" si="4"/>
         <v>1.6089544280900085E-2</v>
       </c>
@@ -3813,7 +3983,7 @@
       <c r="A7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="60">
+      <c r="B7" s="59">
         <v>77.5</v>
       </c>
       <c r="C7" s="48">
@@ -3830,20 +4000,20 @@
         <f>E7/E9</f>
         <v>1.4767974974995133E-3</v>
       </c>
-      <c r="G7" s="66">
+      <c r="G7" s="65">
         <f t="shared" si="3"/>
         <v>1.2075029514221076</v>
       </c>
-      <c r="H7" s="66">
+      <c r="H7" s="65">
         <f t="shared" si="0"/>
         <v>0.20750295142210762</v>
       </c>
-      <c r="I7" s="66">
+      <c r="I7" s="65">
         <f t="shared" si="1"/>
         <v>3.0643983938393159E-4</v>
       </c>
-      <c r="J7" s="66"/>
-      <c r="K7" s="73">
+      <c r="J7" s="65"/>
+      <c r="K7" s="72">
         <f t="shared" si="4"/>
         <v>1.783237336883445E-3</v>
       </c>
@@ -3882,7 +4052,7 @@
         <f>(I8/(I8+1))*100</f>
         <v>1.3486713310096035</v>
       </c>
-      <c r="K8" s="74">
+      <c r="K8" s="73">
         <f>SUM((F2*G2+F3*G3+F4*G4+F5*G5+F6*G6+F7*G7)-1)/(F2*G2+F3*G3+F4*G4+F5*G5+F6*G6+F7*G7)*100</f>
         <v>1.3486713310095881</v>
       </c>
@@ -3944,60 +4114,60 @@
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13"/>
-      <c r="F12" s="70"/>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="71"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="70"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A13" s="112"/>
-      <c r="B13" s="112"/>
-      <c r="C13" s="112"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="70"/>
-      <c r="H13" s="70"/>
-      <c r="I13" s="70"/>
-      <c r="J13" s="70"/>
-      <c r="K13" s="71"/>
+      <c r="A13" s="114"/>
+      <c r="B13" s="114"/>
+      <c r="C13" s="114"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="70"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="113"/>
-      <c r="B14" s="113"/>
-      <c r="C14" s="113"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="K14" s="71"/>
+      <c r="A14" s="115"/>
+      <c r="B14" s="115"/>
+      <c r="C14" s="115"/>
+      <c r="F14" s="71"/>
+      <c r="G14" s="71"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="K14" s="70"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="62"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="56"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="55"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B16" s="8"/>
-      <c r="C16" s="64"/>
+      <c r="C16" s="63"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B17" s="56"/>
-      <c r="C17" s="64"/>
+      <c r="B17" s="55"/>
+      <c r="C17" s="63"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B18" s="8"/>
-      <c r="C18" s="64"/>
+      <c r="C18" s="63"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B19" s="8"/>
-      <c r="C19" s="64"/>
+      <c r="C19" s="63"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="56"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
+      <c r="A20" s="55"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="64"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2"/>
@@ -4006,28 +4176,28 @@
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="7:12" x14ac:dyDescent="0.35">
-      <c r="G34" s="70"/>
-      <c r="H34" s="70"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="71"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="69"/>
+      <c r="L34" s="70"/>
     </row>
     <row r="35" spans="7:12" x14ac:dyDescent="0.35">
-      <c r="G35" s="70"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="70"/>
-      <c r="J35" s="70"/>
-      <c r="K35" s="70"/>
-      <c r="L35" s="71"/>
+      <c r="G35" s="69"/>
+      <c r="H35" s="69"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="69"/>
+      <c r="K35" s="69"/>
+      <c r="L35" s="70"/>
     </row>
     <row r="36" spans="7:12" x14ac:dyDescent="0.35">
-      <c r="G36" s="72"/>
-      <c r="H36" s="72"/>
-      <c r="I36" s="72"/>
-      <c r="J36" s="72"/>
-      <c r="K36" s="72"/>
-      <c r="L36" s="71"/>
+      <c r="G36" s="71"/>
+      <c r="H36" s="71"/>
+      <c r="I36" s="71"/>
+      <c r="J36" s="71"/>
+      <c r="K36" s="71"/>
+      <c r="L36" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4040,54 +4210,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <FHI_TopicTaxHTField xmlns="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Støy</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8f2d7361-ae3f-42e5-b515-973ba07fa140</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Sykdomsbyrde</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">1cb2573e-d91b-47cf-a8ed-abd0332371f0</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Miljø og helse</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">87be7d37-248c-4b3c-9204-980558e4f787</TermId>
-        </TermInfo>
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Miljøeksponering</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">d9196c48-ce51-47cd-b0d2-6ebc45d8709a</TermId>
-        </TermInfo>
-      </Terms>
-    </FHI_TopicTaxHTField>
-    <TaxCatchAll xmlns="e0a242cb-cec1-4671-aa99-615488d5530e">
-      <Value>15</Value>
-      <Value>10</Value>
-      <Value>2</Value>
-      <Value>1</Value>
-    </TaxCatchAll>
-    <TaxKeywordTaxHTField xmlns="e0a242cb-cec1-4671-aa99-615488d5530e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9d23e429-547e-4a13-8b71-070d02c5a1ec">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010000B17EB79AE2164A80F4AFE3B0051146" ma:contentTypeVersion="16" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="6bdb926755f4c89fc32634e0fb424225">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5" xmlns:ns3="e0a242cb-cec1-4671-aa99-615488d5530e" xmlns:ns4="9d23e429-547e-4a13-8b71-070d02c5a1ec" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0d894d6c78ef32a5fd57768bfb40a5e" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5"/>
@@ -4325,27 +4447,55 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA136E82-55D6-4201-8C86-EA83CE955D86}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5"/>
-    <ds:schemaRef ds:uri="e0a242cb-cec1-4671-aa99-615488d5530e"/>
-    <ds:schemaRef ds:uri="9d23e429-547e-4a13-8b71-070d02c5a1ec"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A4E13C-9AD0-4A6A-9D51-20AD50148DE0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <FHI_TopicTaxHTField xmlns="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Støy</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">8f2d7361-ae3f-42e5-b515-973ba07fa140</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Sykdomsbyrde</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">1cb2573e-d91b-47cf-a8ed-abd0332371f0</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Miljø og helse</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">87be7d37-248c-4b3c-9204-980558e4f787</TermId>
+        </TermInfo>
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">Miljøeksponering</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">d9196c48-ce51-47cd-b0d2-6ebc45d8709a</TermId>
+        </TermInfo>
+      </Terms>
+    </FHI_TopicTaxHTField>
+    <TaxCatchAll xmlns="e0a242cb-cec1-4671-aa99-615488d5530e">
+      <Value>15</Value>
+      <Value>10</Value>
+      <Value>2</Value>
+      <Value>1</Value>
+    </TaxCatchAll>
+    <TaxKeywordTaxHTField xmlns="e0a242cb-cec1-4671-aa99-615488d5530e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9d23e429-547e-4a13-8b71-070d02c5a1ec">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AF6BACD-FB0D-4A79-B41F-209A25C08460}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4363,4 +4513,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A4E13C-9AD0-4A6A-9D51-20AD50148DE0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BA136E82-55D6-4201-8C86-EA83CE955D86}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9e7c1b5f-6b93-4ee4-9fa2-fda8f1b47cf5"/>
+    <ds:schemaRef ds:uri="e0a242cb-cec1-4671-aa99-615488d5530e"/>
+    <ds:schemaRef ds:uri="9d23e429-547e-4a13-8b71-070d02c5a1ec"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>